<commit_message>
Update output (not showing answers)
</commit_message>
<xml_diff>
--- a/quiz.xlsx
+++ b/quiz.xlsx
@@ -12,21 +12,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Quiz</t>
+  </si>
+  <si>
+    <t>Excel-quiz</t>
+  </si>
+  <si>
+    <t>Question 1</t>
   </si>
   <si>
     <t>Where do you find the best answers?</t>
   </si>
   <si>
-    <t>Stack-Overflow</t>
+    <t>Question 2</t>
   </si>
   <si>
     <t>Who to ask?</t>
-  </si>
-  <si>
-    <t>mwb</t>
   </si>
 </sst>
 </file>
@@ -82,19 +85,21 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2"/>
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>